<commit_message>
My 9th commit through Intellij
</commit_message>
<xml_diff>
--- a/target/classes/NinzaData.xlsx
+++ b/target/classes/NinzaData.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shekhar\IdeaProjects\SeleniumDemo\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4E4780-8C6F-4D98-96E3-E975C06D7641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="NinzaAutomation" r:id="rId5" sheetId="2"/>
+    <sheet name="Campaigns" sheetId="3" r:id="rId1"/>
+    <sheet name="Contacts" sheetId="1" r:id="rId2"/>
+    <sheet name="Products" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,19 +27,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Price</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Contact Name</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>PricePerUnit</t>
+  </si>
+  <si>
+    <t>CampaignName</t>
+  </si>
+  <si>
+    <t>TargetSize</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Qspiders-4510</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -62,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,34 +383,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C909008-88EA-4978-8FFF-642A196DACDE}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="F6:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="6">
-      <c r="F6" t="s" s="0">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="G6" t="s" s="0">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AF93B0-89C6-4514-BC90-A49869839BD3}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>